<commit_message>
addd type di tahapan
</commit_message>
<xml_diff>
--- a/public/templates/import_pengadaan_template.xlsx
+++ b/public/templates/import_pengadaan_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pln-laravel\public\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\monitoring-api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE85317-984D-4780-8B16-6D779A1D6179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6D4D6B-F429-4B33-9AC0-A37E27F2AE87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2505" windowWidth="15375" windowHeight="7995" xr2:uid="{40E8CDBE-C041-4AF3-8CAE-C0C1B20AB6A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{40E8CDBE-C041-4AF3-8CAE-C0C1B20AB6A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maul</author>
+    <author>Ichwan</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{802F5F66-BB26-4E69-8E90-8DFF4A9D0F4A}">
@@ -78,7 +79,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{303C848A-C8DC-477E-A5C5-D6760FD59ECB}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{B1A16056-70CA-4F47-B366-1EE9705C1DB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MURNI
+LUNCURAN</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{303C848A-C8DC-477E-A5C5-D6760FD59ECB}">
       <text>
         <r>
           <rPr>
@@ -93,12 +109,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{B89E9F58-5CC1-4ECD-BCD0-AD540A68AA53}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jika lebih dari 1 PRK-SKKI, pisahkan dengan ;</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Basket</t>
   </si>
@@ -109,13 +139,19 @@
     <t>Tanggal Nodin</t>
   </si>
   <si>
-    <t>PR</t>
-  </si>
-  <si>
     <t>Nama Project</t>
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>PR Jasa</t>
+  </si>
+  <si>
+    <t>Tipe</t>
+  </si>
+  <si>
+    <t>PRK-SKKI</t>
   </si>
 </sst>
 </file>
@@ -475,18 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAAA200-6412-4E12-B322-CF7E891DADE0}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -494,19 +531,25 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
   </sheetData>

</xml_diff>